<commit_message>
functional database json and excel files generated
</commit_message>
<xml_diff>
--- a/database/1hs.xlsx
+++ b/database/1hs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Recipe</t>
+          <t>Processing</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recipes</t>
         </is>
       </c>
     </row>
@@ -463,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Stat/EffectAmountATK %
+          <t>ATK %
 11
 Stability %
 10
@@ -489,6 +494,387 @@
           <t>Sell0 SpinaProcessunknown</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Anguish Sword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ATK %
+11
+Stability %
+10
+Physical Pierce %
+20
+ASPD
+900
+%
+stronger against Light
+10
+Dark Element
+0
+Guard Break %30</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[NPC]Blacksmith : ZaldoSofya City: Blacksmith</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Sell0 SpinaProcessunknown</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Anguish Sword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ATK %
+11
+Stability %
+10
+Physical Pierce %
+20
+ASPD
+900
+%
+stronger against Light
+10
+Dark Element
+0
+Guard Break %30</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>empty</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Sell0 SpinaProcessunknown</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Accordion-fold Sword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Base ATK
+1
+Aggro %
+30
+Attack MP Recovery
+3
+Base Stability %40</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>[NPC]Blacksmith : ZaldoSofya City: Blacksmith</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>SellUnknownProcessN/A</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Fee
+150
+ SpinaSet
+1
+ pcsLevelN/ADifficulty
+0
+Materials- 
+25
+xBat Wing- 
+1
+xFour-leaf Clover- 
+50
+x Cloth- 
+25
+x Metal</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Shortsword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Base ATK
+10
+Base Stability %80</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Pico(Lv 1)Rakau Plains</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Sell1 SpinaProcess2 Metal</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Shortsword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Base ATK
+10
+Base Stability %80</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[NPC]Blacksmith : ZaldoSofya City: Blacksmith</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sell1 SpinaProcess2 Metal</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Fee
+5
+ SpinaSet
+1
+ pcsLevel
+1
+Difficulty
+1
+Materials- 
+3
+x Metal</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Shortsword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Base ATK
+10
+Base Stability %
+80
+Potential15</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[Player]Smith Skill-</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Sell1 SpinaProcess2 Metal</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Fee
+5
+ SpinaSet
+1
+ pcsLevel
+1
+Difficulty
+1
+Materials- 
+3
+x Metal</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Wood Sword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Base ATK
+10
+Base Stability %
+40
+Potential15</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[Player]Smith Skill-</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sell1 SpinaProcess2 Wood</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>FeeN/ASet
+1
+ pcsLevel
+1
+Difficulty
+0
+Materials- 
+25
+x Wood</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Longsword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Base ATK
+17
+MaxHP
+50
+Accuracy
+1
+Base Stability %80</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[NPC]Blacksmith : ZaldoSofya City: Blacksmith</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Sell10 SpinaProcess5 Metal</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Fee
+50
+ SpinaSet
+1
+ pcsLevel
+5
+Difficulty
+10
+Materials- 
+20
+xSmall Hilt- 
+25
+x Metal</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Longsword[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Base ATK
+17
+Base Stability %
+80
+Potential16</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[Player]Smith Skill-</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Sell10 SpinaProcess5 Metal</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Fee
+50
+ SpinaSet
+1
+ pcsLevel
+5
+Difficulty
+10
+Materials- 
+20
+xSmall Hilt- 
+25
+x Metal</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Gladius[1 Handed Sword]</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Base ATK
+25
+ASPD %
+5
+Critical Rate
+1
+Base Stability %80</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Goblin(Lv 20)Ruined Temple: Area 1Goblin(Lv 20)Ruined Temple: Area 2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Sell20 SpinaProcess10 Metal</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>